<commit_message>
different method of reading file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>key</t>
   </si>
@@ -26,6 +27,42 @@
   </si>
   <si>
     <t>orangutan</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>passport no</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>anthony</t>
+  </si>
+  <si>
+    <t>a34214234</t>
+  </si>
+  <si>
+    <t>jegede street 23, opp owners occupiers</t>
+  </si>
+  <si>
+    <t>okoli</t>
+  </si>
+  <si>
+    <t>r43242424</t>
+  </si>
+  <si>
+    <t>street gonduro, appartment 34</t>
+  </si>
+  <si>
+    <t>dud</t>
+  </si>
+  <si>
+    <t>f77200033</t>
+  </si>
+  <si>
+    <t>makuerdi express, room 545</t>
   </si>
 </sst>
 </file>
@@ -78,6 +115,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
@@ -120,4 +161,63 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="11.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>